<commit_message>
added the robot-assets valkyrie model
</commit_message>
<xml_diff>
--- a/robot_types.xlsx
+++ b/robot_types.xlsx
@@ -5,28 +5,29 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://connectqutedu-my.sharepoint.com/personal/tola_qut_edu_au/Documents/Desktop/gitrepos/urdf_files_dataset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://connectqutedu-my.sharepoint.com/personal/tola_qut_edu_au/Documents/Desktop/gitrepos/urdf_analyzer/resources/urdf_files_dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="844" documentId="11_F25DC773A252ABDACC104829591E5E145ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE7732A7-AAB3-4C90-806D-77CC987081B1}"/>
+  <xr:revisionPtr revIDLastSave="859" documentId="11_F25DC773A252ABDACC104829591E5E145ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EA9F2E5-8730-4FE3-AE14-CCD58CD97EED}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classification" sheetId="1" r:id="rId1"/>
     <sheet name="duplicates" sheetId="4" r:id="rId2"/>
     <sheet name="urdf from manufacturers" sheetId="5" r:id="rId3"/>
-    <sheet name="comparison with urdf from OEM" sheetId="6" r:id="rId4"/>
-    <sheet name="information" sheetId="2" r:id="rId5"/>
-    <sheet name="analysis" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId4"/>
+    <sheet name="comparison with urdf from OEM" sheetId="6" r:id="rId5"/>
+    <sheet name="information" sheetId="2" r:id="rId6"/>
+    <sheet name="analysis" sheetId="3" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'urdf from manufacturers'!$A$1:$B$81</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId7"/>
-    <pivotCache cacheId="1" r:id="rId8"/>
+    <pivotCache cacheId="0" r:id="rId8"/>
+    <pivotCache cacheId="1" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="178">
   <si>
     <t>Robot</t>
   </si>
@@ -7556,6 +7557,162 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7F910A06-381E-4205-8A11-C037FFB06F19}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A25:B30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="3"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Type" fld="1" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BC3F2483-E8BF-4DBF-A164-60FE6E5E2B6B}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A3:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="11">
+        <item x="5"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="7"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Type" fld="1" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C8D76A50-2177-495E-9784-C4DC095E567F}" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A83:E109" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="2">
@@ -7744,7 +7901,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{52084291-B8D7-48BB-BE93-50F506D1CFF2}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A48:F74" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
@@ -8217,162 +8374,6 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7F910A06-381E-4205-8A11-C037FFB06F19}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A25:B30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="4">
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item x="3"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Type" fld="1" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BC3F2483-E8BF-4DBF-A164-60FE6E5E2B6B}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A3:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="4">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="11">
-        <item x="5"/>
-        <item x="1"/>
-        <item x="6"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="7"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="11">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Type" fld="1" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -8638,8 +8639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10510,15 +10511,11 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="F18:F19"/>
     <mergeCell ref="G12:G13"/>
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="F2:F3"/>
@@ -10532,11 +10529,15 @@
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="G10:G11"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H10:H11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10565,8 +10566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE66FBE9-F7B0-4854-A23C-4A71EF1A3A3A}">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10606,16 +10607,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -10645,251 +10643,254 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>143</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
         <v>135</v>
       </c>
+      <c r="D6" s="7" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="E7" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C8" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="E8" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
         <v>135</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>149</v>
+      <c r="D9" s="6" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>143</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="C11" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
         <v>135</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>151</v>
-      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="C13" t="s">
-        <v>143</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="C16" t="s">
-        <v>135</v>
+        <v>143</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E16" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>124</v>
       </c>
       <c r="B17" t="s">
-        <v>106</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
-        <v>135</v>
+        <v>143</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="E17" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C18" t="s">
-        <v>135</v>
+        <v>143</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C19" t="s">
         <v>143</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="E19" t="s">
-        <v>165</v>
-      </c>
-      <c r="F19" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>116</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C20" t="s">
         <v>143</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
+      </c>
+      <c r="E20" t="s">
+        <v>165</v>
+      </c>
+      <c r="F20" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C21" t="s">
         <v>143</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="E21" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C22" t="s">
-        <v>135</v>
+        <v>143</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E22" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -10943,22 +10944,30 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G25">
+    <sortCondition ref="C2:C25"/>
+  </sortState>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C25" xr:uid="{1AF688A6-E6CD-4C08-9181-ACF0DEB89626}">
+      <formula1>"Yes,No,N/A"</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{BD6B94F4-06B9-4404-A468-60E25E6425F0}"/>
-    <hyperlink ref="D5" r:id="rId2" xr:uid="{7D909D3A-1245-49CE-B04F-A449605E512B}"/>
-    <hyperlink ref="D7" r:id="rId3" xr:uid="{991712BE-2DAB-433E-B7F1-1736F0FA63FA}"/>
-    <hyperlink ref="D8" r:id="rId4" xr:uid="{7F9BDFFC-91E2-4241-B41B-C17461E2C2B4}"/>
-    <hyperlink ref="D10" r:id="rId5" xr:uid="{6F8FA59F-CEBE-440C-B910-037FB9729522}"/>
-    <hyperlink ref="D12" r:id="rId6" xr:uid="{05D694FD-20A6-4331-BA72-F002408A4734}"/>
-    <hyperlink ref="D13" r:id="rId7" xr:uid="{1249D900-31C7-47D0-A0CF-0F709CA92A3C}"/>
-    <hyperlink ref="D14" r:id="rId8" xr:uid="{4FA17220-086F-4CCC-A67F-A03213DF3CDC}"/>
-    <hyperlink ref="D15" r:id="rId9" xr:uid="{406FB329-6AB5-4462-9EA4-C8714AC37DC3}"/>
-    <hyperlink ref="D19" r:id="rId10" xr:uid="{DA06B138-B937-4E20-B62E-A90FAC325B11}"/>
-    <hyperlink ref="D20" r:id="rId11" xr:uid="{A62C92FB-C8D8-46D9-AB42-E372679F073E}"/>
-    <hyperlink ref="D21" r:id="rId12" xr:uid="{42F3A13A-56A9-4791-B05C-CBB1DFCDCFCC}"/>
-    <hyperlink ref="D23" r:id="rId13" xr:uid="{EAC90D7E-B3CB-42E5-80E2-92A373E1A09B}"/>
-    <hyperlink ref="D24" r:id="rId14" xr:uid="{1C66CEB9-4876-4BB8-A432-02FAE1D5C3BD}"/>
-    <hyperlink ref="D25" r:id="rId15" xr:uid="{016D0BC9-FC83-424E-AD4C-F36D6AF1414E}"/>
+    <hyperlink ref="D14" r:id="rId1" xr:uid="{BD6B94F4-06B9-4404-A468-60E25E6425F0}"/>
+    <hyperlink ref="D15" r:id="rId2" xr:uid="{7D909D3A-1245-49CE-B04F-A449605E512B}"/>
+    <hyperlink ref="D16" r:id="rId3" xr:uid="{991712BE-2DAB-433E-B7F1-1736F0FA63FA}"/>
+    <hyperlink ref="D17" r:id="rId4" xr:uid="{7F9BDFFC-91E2-4241-B41B-C17461E2C2B4}"/>
+    <hyperlink ref="D18" r:id="rId5" xr:uid="{6F8FA59F-CEBE-440C-B910-037FB9729522}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{05D694FD-20A6-4331-BA72-F002408A4734}"/>
+    <hyperlink ref="D19" r:id="rId7" xr:uid="{1249D900-31C7-47D0-A0CF-0F709CA92A3C}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{406FB329-6AB5-4462-9EA4-C8714AC37DC3}"/>
+    <hyperlink ref="D20" r:id="rId9" xr:uid="{DA06B138-B937-4E20-B62E-A90FAC325B11}"/>
+    <hyperlink ref="D21" r:id="rId10" xr:uid="{A62C92FB-C8D8-46D9-AB42-E372679F073E}"/>
+    <hyperlink ref="D22" r:id="rId11" xr:uid="{42F3A13A-56A9-4791-B05C-CBB1DFCDCFCC}"/>
+    <hyperlink ref="D23" r:id="rId12" xr:uid="{EAC90D7E-B3CB-42E5-80E2-92A373E1A09B}"/>
+    <hyperlink ref="D24" r:id="rId13" xr:uid="{1C66CEB9-4876-4BB8-A432-02FAE1D5C3BD}"/>
+    <hyperlink ref="D25" r:id="rId14" xr:uid="{016D0BC9-FC83-424E-AD4C-F36D6AF1414E}"/>
+    <hyperlink ref="D8" r:id="rId15" xr:uid="{4FA17220-086F-4CCC-A67F-A03213DF3CDC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
@@ -10967,11 +10976,404 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692F1E00-39BF-476A-BCE7-7C5C3DDA9644}">
+  <dimension ref="A1:G25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" t="s">
+        <v>143</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="300" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>143</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" t="s">
+        <v>135</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C17" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" t="s">
+        <v>143</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="E19" t="s">
+        <v>165</v>
+      </c>
+      <c r="F19" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" t="s">
+        <v>143</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" t="s">
+        <v>143</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E21" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" t="s">
+        <v>143</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" t="s">
+        <v>143</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" t="s">
+        <v>143</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="E25" t="s">
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C25" xr:uid="{3AE8E020-5AC8-4DB7-A682-789624970DFC}">
+      <formula1>"Yes,No,N/A"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{163A4CF0-999A-45BC-9AAF-D653049319DB}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{B8BF1BAE-C82C-45B9-9EE7-A7545F9302C4}"/>
+    <hyperlink ref="D7" r:id="rId3" xr:uid="{7F002BDA-CBD2-46CD-B51F-A4634D97C27B}"/>
+    <hyperlink ref="D8" r:id="rId4" xr:uid="{9680EB78-C85F-40C8-BE31-9C80403A7720}"/>
+    <hyperlink ref="D10" r:id="rId5" xr:uid="{B775B6C7-11A7-43E6-8597-363B04B44A53}"/>
+    <hyperlink ref="D12" r:id="rId6" xr:uid="{D4192AFD-D948-4BBD-BB5C-2C5C00316084}"/>
+    <hyperlink ref="D13" r:id="rId7" xr:uid="{E59F24E0-A6EC-4383-89E2-E54D78C38EED}"/>
+    <hyperlink ref="D15" r:id="rId8" xr:uid="{AFCB51B5-F31A-4A43-A53B-243B15B309E1}"/>
+    <hyperlink ref="D19" r:id="rId9" xr:uid="{FC3C92EE-628D-4A54-8B71-80EADDED16E8}"/>
+    <hyperlink ref="D20" r:id="rId10" xr:uid="{CAEF8583-305E-4727-8574-D403418B719E}"/>
+    <hyperlink ref="D21" r:id="rId11" xr:uid="{063B48E2-5EA3-433F-A07F-2018D56B1C19}"/>
+    <hyperlink ref="D23" r:id="rId12" xr:uid="{3A4B39B7-E78F-489A-AECE-C8EBF1DB74DC}"/>
+    <hyperlink ref="D24" r:id="rId13" xr:uid="{BD5BC50A-4945-40A0-9CE3-0CA102749363}"/>
+    <hyperlink ref="D25" r:id="rId14" xr:uid="{C4C1F6D9-C281-4582-96F2-481D4F7D8F07}"/>
+    <hyperlink ref="D14" r:id="rId15" xr:uid="{5C8FCB42-03C1-4E9F-99BF-2C31CF060E17}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71FD75EA-32EE-428F-89A7-E3503ACE3CA3}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11117,7 +11519,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D436AF-4A5C-4F46-81DF-CC60230C3571}">
   <dimension ref="A1:B12"/>
   <sheetViews>
@@ -11212,7 +11614,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BABF643E-67AC-4C76-84C9-66392C75839F}">
   <dimension ref="A3:F109"/>
   <sheetViews>

</xml_diff>

<commit_message>
added kinova and franka urdf files generated from xacro
</commit_message>
<xml_diff>
--- a/robot_types.xlsx
+++ b/robot_types.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://connectqutedu-my.sharepoint.com/personal/tola_qut_edu_au/Documents/Desktop/gitrepos/urdf_analyzer/resources/urdf_files_dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="859" documentId="11_F25DC773A252ABDACC104829591E5E145ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EA9F2E5-8730-4FE3-AE14-CCD58CD97EED}"/>
+  <xr:revisionPtr revIDLastSave="867" documentId="11_F25DC773A252ABDACC104829591E5E145ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5391DEC-F350-4660-9B28-3B4E34555DD8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10511,11 +10511,15 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H10:H11"/>
     <mergeCell ref="G12:G13"/>
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="F2:F3"/>
@@ -10529,15 +10533,11 @@
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="F18:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10567,7 +10567,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10979,11 +10979,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692F1E00-39BF-476A-BCE7-7C5C3DDA9644}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G25"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" customWidth="1"/>
+    <col min="3" max="3" width="39.85546875" customWidth="1"/>
+    <col min="4" max="4" width="77.28515625" customWidth="1"/>
+    <col min="5" max="5" width="40.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
updated with xacro generated urdf files from oems
</commit_message>
<xml_diff>
--- a/robot_types.xlsx
+++ b/robot_types.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://connectqutedu-my.sharepoint.com/personal/tola_qut_edu_au/Documents/Desktop/gitrepos/urdf_analyzer/resources/urdf_files_dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="867" documentId="11_F25DC773A252ABDACC104829591E5E145ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5391DEC-F350-4660-9B28-3B4E34555DD8}"/>
+  <xr:revisionPtr revIDLastSave="949" documentId="11_F25DC773A252ABDACC104829591E5E145ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9484EC17-7D4B-4FDC-9726-9954343F4A04}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classification" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,8 @@
   <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId8"/>
-    <pivotCache cacheId="1" r:id="rId9"/>
+    <pivotCache cacheId="9" r:id="rId9"/>
+    <pivotCache cacheId="14" r:id="rId10"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="181">
   <si>
     <t>Robot</t>
   </si>
@@ -360,9 +361,6 @@
     <t>Kinova Jaco Two Arm Example</t>
   </si>
   <si>
-    <t>Kinova Mico M1N2S200</t>
-  </si>
-  <si>
     <t>Kinova Mico M1N6S200</t>
   </si>
   <si>
@@ -583,6 +581,18 @@
   </si>
   <si>
     <t>eve R3</t>
+  </si>
+  <si>
+    <t>spot</t>
+  </si>
+  <si>
+    <t>Accessed</t>
+  </si>
+  <si>
+    <t>Count of Accessed</t>
+  </si>
+  <si>
+    <t>Kinova Mico M1N4S200</t>
   </si>
 </sst>
 </file>
@@ -661,7 +671,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -680,6 +690,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -6698,8 +6709,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2973169</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>170098</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>19212</xdr:rowOff>
     </xdr:to>
@@ -6921,34 +6932,34 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Daniella Tola" refreshedDate="44855.549729976854" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="24" xr:uid="{9B0CFF11-C190-42A6-A3F0-43EBAC7C32E2}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Daniella Tola" refreshedDate="44873.448786458335" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="24" xr:uid="{9B0CFF11-C190-42A6-A3F0-43EBAC7C32E2}">
   <cacheSource type="worksheet">
     <worksheetSource ref="B1:C25" sheet="urdf from manufacturers"/>
   </cacheSource>
   <cacheFields count="2">
     <cacheField name="Manufacturer" numFmtId="0">
       <sharedItems count="24">
-        <s v="ANYbotics"/>
+        <s v="Fictitious character"/>
         <s v="Barret Technology"/>
         <s v="Fetch Robotics"/>
-        <s v="Franka Emika"/>
         <s v="Paaila Technology"/>
-        <s v="Halodi Robotics"/>
-        <s v="Kinova Robotics"/>
         <s v="kuka"/>
-        <s v="Willow Garage"/>
-        <s v="Fictitious character"/>
         <s v="robotiq"/>
-        <s v="universal robots"/>
         <s v="NASA"/>
         <s v="abb"/>
         <s v="schunk"/>
         <s v="Yaskawa Motoman Robotics"/>
         <s v="staubli"/>
+        <s v="Fanuc"/>
+        <s v="ANYbotics"/>
+        <s v="Franka Emika"/>
+        <s v="Halodi Robotics"/>
+        <s v="Kinova Robotics"/>
+        <s v="Willow Garage"/>
+        <s v="universal robots"/>
         <s v="Adept MobileRobots"/>
         <s v="Boston Dynamics"/>
         <s v="Rethink Robotics"/>
-        <s v="Fanuc"/>
         <s v="Clearpath robotics"/>
         <s v="Robotis"/>
         <s v="Quanser"/>
@@ -6956,10 +6967,79 @@
     </cacheField>
     <cacheField name="Manufacturer provides URDF file" numFmtId="0">
       <sharedItems count="3">
+        <s v="N/A"/>
+        <s v="No"/>
         <s v="Yes"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Daniella Tola" refreshedDate="44873.449190509258" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="24" xr:uid="{15D6D7DD-31E2-4D2E-A142-53491CCF7478}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:G25" sheet="urdf from manufacturers"/>
+  </cacheSource>
+  <cacheFields count="7">
+    <cacheField name="Robot" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Manufacturer" numFmtId="0">
+      <sharedItems count="24">
+        <s v="Fictitious character"/>
+        <s v="Barret Technology"/>
+        <s v="Fetch Robotics"/>
+        <s v="Paaila Technology"/>
+        <s v="kuka"/>
+        <s v="robotiq"/>
+        <s v="NASA"/>
+        <s v="abb"/>
+        <s v="schunk"/>
+        <s v="Yaskawa Motoman Robotics"/>
+        <s v="staubli"/>
+        <s v="Fanuc"/>
+        <s v="ANYbotics"/>
+        <s v="Franka Emika"/>
+        <s v="Halodi Robotics"/>
+        <s v="Kinova Robotics"/>
+        <s v="Willow Garage"/>
+        <s v="universal robots"/>
+        <s v="Adept MobileRobots"/>
+        <s v="Boston Dynamics"/>
+        <s v="Rethink Robotics"/>
+        <s v="Clearpath robotics"/>
+        <s v="Robotis"/>
+        <s v="Quanser"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Manufacturer provides URDF file" numFmtId="0">
+      <sharedItems count="3">
+        <s v="N/A"/>
         <s v="No"/>
+        <s v="Yes"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Accessed" numFmtId="0">
+      <sharedItems count="3">
         <s v="N/A"/>
+        <s v="No"/>
+        <s v="Yes"/>
       </sharedItems>
+    </cacheField>
+    <cacheField name="Where" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Last modified" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Interesting comments in urdfs" numFmtId="0">
+      <sharedItems containsBlank="1"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -7471,7 +7551,7 @@
   </r>
   <r>
     <x v="3"/>
-    <x v="0"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="4"/>
@@ -7479,11 +7559,11 @@
   </r>
   <r>
     <x v="5"/>
-    <x v="0"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="6"/>
-    <x v="0"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="7"/>
@@ -7491,11 +7571,11 @@
   </r>
   <r>
     <x v="8"/>
-    <x v="0"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="9"/>
-    <x v="2"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="10"/>
@@ -7503,60 +7583,470 @@
   </r>
   <r>
     <x v="11"/>
-    <x v="0"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="12"/>
-    <x v="1"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="13"/>
-    <x v="1"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="14"/>
-    <x v="1"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="15"/>
-    <x v="1"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="16"/>
-    <x v="1"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="17"/>
-    <x v="0"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="18"/>
-    <x v="0"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="19"/>
-    <x v="0"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="20"/>
-    <x v="1"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="21"/>
-    <x v="0"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="22"/>
-    <x v="0"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="23"/>
+    <x v="2"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="24">
+  <r>
+    <s v="R2D2"/>
     <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="Barret hand"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="Fetch"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="but relevant descriptions"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="Ginger robot"/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="Kuka iiwa"/>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="https://github.com/kuka-isir/iiwa_description and https://gitlab.kuleuven.be/r0597555/iiwa_stack/-/tree/636f3dfc47f4d88f097a907f38868b6f1f3efb5f/iiwa_description "/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="Robotiq gripper arg85"/>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="https://github.com/ros-industrial/robotiq "/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="valkyrie"/>
+    <x v="6"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="https://github.com/gkjohnson/nasa-urdf-robots "/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="yumi"/>
+    <x v="7"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="https://github.com/ros-industrial/abb "/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="schunk lwa4p"/>
+    <x v="8"/>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="motoman mh5"/>
+    <x v="9"/>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="rx 160"/>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="lr mate 200ib"/>
+    <x v="11"/>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="ANYmal"/>
+    <x v="12"/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="https://github.com/ANYbotics/anymal_b_simple_description "/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="Franka panda"/>
+    <x v="13"/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="https://github.com/frankaemika/franka_ros/tree/develop/franka_description "/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="Halodi"/>
+    <x v="14"/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="https://github.com/Halodi/halodi-robot-models/tree/main/eve_r3_description "/>
+    <s v="9 months ago"/>
+    <m/>
+  </r>
+  <r>
+    <s v="Kinova Jaco AnyMAL bedi"/>
+    <x v="15"/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="https://github.com/Kinovarobotics/kinova-ros/tree/melodic-devel/kinova_description "/>
+    <s v="11 months ago"/>
+    <m/>
+  </r>
+  <r>
+    <s v="PR2"/>
+    <x v="16"/>
+    <x v="2"/>
+    <x v="1"/>
+    <s v="https://github.com/PR2/pr2_common/tree/melodic-devel/pr2_description "/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="ur5"/>
+    <x v="17"/>
+    <x v="2"/>
+    <x v="1"/>
+    <s v="https://github.com/UniversalRobots/Universal_Robots_ROS2_Description "/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="amr pioneer 3AT"/>
+    <x v="18"/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="https://github.com/MobileRobots/amr-ros-config/tree/master/description "/>
+    <s v="6 years ago"/>
+    <s v="TODO"/>
+  </r>
+  <r>
+    <s v="spot"/>
+    <x v="19"/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="https://dev.bostondynamics.com/docs/concepts/robot_services "/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="baxter"/>
+    <x v="20"/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="https://github.com/RethinkRobotics/baxter_common/tree/master/baxter_description "/>
+    <s v="7 years ago"/>
+    <m/>
+  </r>
+  <r>
+    <s v="Jackal"/>
+    <x v="21"/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="https://www.clearpathrobotics.com/assets/guides/kinetic/jackal/description.html "/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="Open manipulator"/>
+    <x v="22"/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="https://github.com/ROBOTIS-GIT/open_manipulator/tree/master/open_manipulator_description "/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="Quanser QArm"/>
+    <x v="23"/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="https://github.com/quanser/qarm_description "/>
+    <s v="2 years ago"/>
+    <m/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7DB9AB06-7A0B-43D1-8D65-CBF8CDFF313F}" name="PivotTable6" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A125:B129" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="25">
+        <item x="7"/>
+        <item x="18"/>
+        <item x="12"/>
+        <item x="1"/>
+        <item x="19"/>
+        <item x="21"/>
+        <item x="11"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item x="3"/>
+        <item x="23"/>
+        <item x="20"/>
+        <item x="5"/>
+        <item x="22"/>
+        <item x="8"/>
+        <item x="10"/>
+        <item x="17"/>
+        <item x="16"/>
+        <item x="9"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Manufacturer provides URDF file" fld="2" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7247F8BF-CB69-45E8-B510-8C11315D1775}" name="PivotTable5" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A116:B120" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="25">
+        <item x="7"/>
+        <item x="18"/>
+        <item x="12"/>
+        <item x="1"/>
+        <item x="19"/>
+        <item x="21"/>
+        <item x="11"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item x="3"/>
+        <item x="23"/>
+        <item x="20"/>
+        <item x="5"/>
+        <item x="22"/>
+        <item x="8"/>
+        <item x="10"/>
+        <item x="17"/>
+        <item x="16"/>
+        <item x="9"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Accessed" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="37" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7F910A06-381E-4205-8A11-C037FFB06F19}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A25:B30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
@@ -7622,7 +8112,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BC3F2483-E8BF-4DBF-A164-60FE6E5E2B6B}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
@@ -7712,44 +8202,44 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C8D76A50-2177-495E-9784-C4DC095E567F}" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C8D76A50-2177-495E-9784-C4DC095E567F}" name="PivotTable4" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A83:E109" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
       <items count="25">
+        <item x="7"/>
+        <item x="18"/>
+        <item x="12"/>
+        <item x="1"/>
+        <item x="19"/>
+        <item x="21"/>
+        <item x="11"/>
+        <item x="2"/>
+        <item x="0"/>
         <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item x="3"/>
+        <item x="23"/>
+        <item x="20"/>
+        <item x="5"/>
+        <item x="22"/>
+        <item x="8"/>
+        <item x="10"/>
         <item x="17"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="18"/>
-        <item x="21"/>
-        <item x="20"/>
-        <item x="2"/>
+        <item x="16"/>
         <item x="9"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="12"/>
-        <item x="4"/>
-        <item x="23"/>
-        <item x="19"/>
-        <item x="10"/>
-        <item x="22"/>
-        <item x="14"/>
-        <item x="16"/>
-        <item x="11"/>
-        <item x="8"/>
-        <item x="15"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisCol" dataField="1" showAll="0">
       <items count="4">
+        <item x="0"/>
+        <item x="1"/>
         <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -7901,7 +8391,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{52084291-B8D7-48BB-BE93-50F506D1CFF2}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A48:F74" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
@@ -8639,8 +9129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8773,10 +9263,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C8" t="s">
         <v>23</v>
@@ -8824,7 +9314,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
@@ -9088,7 +9578,7 @@
         <v>26</v>
       </c>
       <c r="D26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -9105,7 +9595,7 @@
         <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -9122,7 +9612,7 @@
         <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -9139,7 +9629,7 @@
         <v>26</v>
       </c>
       <c r="D29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -9156,7 +9646,7 @@
         <v>26</v>
       </c>
       <c r="D30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -9266,7 +9756,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B37" t="s">
         <v>18</v>
@@ -9300,7 +9790,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B39" t="s">
         <v>67</v>
@@ -9317,7 +9807,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B40" t="s">
         <v>67</v>
@@ -9334,7 +9824,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B41" t="s">
         <v>67</v>
@@ -9453,7 +9943,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B48" t="s">
         <v>18</v>
@@ -9470,7 +9960,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B49" t="s">
         <v>18</v>
@@ -9606,7 +10096,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>103</v>
+        <v>180</v>
       </c>
       <c r="B57" t="s">
         <v>90</v>
@@ -9623,7 +10113,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B58" t="s">
         <v>90</v>
@@ -9640,7 +10130,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B59" t="s">
         <v>98</v>
@@ -9700,7 +10190,7 @@
         <v>28</v>
       </c>
       <c r="D62" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -9759,7 +10249,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B66" t="s">
         <v>18</v>
@@ -9776,7 +10266,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B67" t="s">
         <v>67</v>
@@ -9793,7 +10283,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B68" t="s">
         <v>67</v>
@@ -9844,7 +10334,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B71" t="s">
         <v>67</v>
@@ -9861,7 +10351,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B72" t="s">
         <v>67</v>
@@ -9878,7 +10368,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B73" t="s">
         <v>67</v>
@@ -9895,7 +10385,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B74" t="s">
         <v>67</v>
@@ -9912,7 +10402,7 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B75" t="s">
         <v>67</v>
@@ -9929,7 +10419,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B76" t="s">
         <v>67</v>
@@ -10090,13 +10580,13 @@
         <v>95</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -10116,13 +10606,13 @@
         <v>1</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -10162,13 +10652,13 @@
         <v>1</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -10208,10 +10698,10 @@
         <v>1</v>
       </c>
       <c r="F6" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="G6" s="9" t="s">
         <v>125</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>126</v>
       </c>
       <c r="H6" s="9"/>
     </row>
@@ -10252,13 +10742,13 @@
         <v>1</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -10298,18 +10788,18 @@
         <v>1</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>18</v>
@@ -10329,7 +10819,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>18</v>
@@ -10344,13 +10834,13 @@
         <v>1</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -10384,19 +10874,19 @@
         <v>26</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E14" s="4">
         <v>1</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -10410,7 +10900,7 @@
         <v>28</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E15" s="4">
         <v>1</v>
@@ -10436,13 +10926,13 @@
         <v>1</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -10482,10 +10972,10 @@
         <v>1</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H18" s="9"/>
     </row>
@@ -10511,15 +11001,11 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="F18:F19"/>
     <mergeCell ref="G12:G13"/>
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="F2:F3"/>
@@ -10533,11 +11019,15 @@
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="G10:G11"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H10:H11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10566,8 +11056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE66FBE9-F7B0-4854-A23C-4A71EF1A3A3A}">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10575,7 +11065,7 @@
     <col min="1" max="1" width="31.85546875" customWidth="1"/>
     <col min="2" max="2" width="35.140625" customWidth="1"/>
     <col min="3" max="3" width="35.5703125" customWidth="1"/>
-    <col min="4" max="4" width="88.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
     <col min="5" max="5" width="27.7109375" customWidth="1"/>
     <col min="6" max="6" width="29.85546875" customWidth="1"/>
     <col min="7" max="7" width="29" customWidth="1"/>
@@ -10589,31 +11079,36 @@
         <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>144</v>
+        <v>178</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
         <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>142</v>
+        <v>141</v>
+      </c>
+      <c r="D2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -10624,7 +11119,10 @@
         <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>135</v>
+        <v>134</v>
+      </c>
+      <c r="D3" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -10635,10 +11133,13 @@
         <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D4" t="s">
-        <v>159</v>
+        <v>134</v>
+      </c>
+      <c r="E4" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -10649,10 +11150,13 @@
         <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="D5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -10660,10 +11164,13 @@
         <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>135</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>149</v>
+        <v>134</v>
+      </c>
+      <c r="D6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -10674,10 +11181,13 @@
         <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>135</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>151</v>
+        <v>134</v>
+      </c>
+      <c r="D7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -10688,13 +11198,16 @@
         <v>64</v>
       </c>
       <c r="C8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="D8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -10702,10 +11215,13 @@
         <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>135</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>154</v>
+        <v>134</v>
+      </c>
+      <c r="D9" t="s">
+        <v>134</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -10716,7 +11232,10 @@
         <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>135</v>
+        <v>134</v>
+      </c>
+      <c r="D10" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -10724,10 +11243,13 @@
         <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C11" t="s">
-        <v>135</v>
+        <v>134</v>
+      </c>
+      <c r="D11" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -10738,7 +11260,10 @@
         <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>135</v>
+        <v>134</v>
+      </c>
+      <c r="D12" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -10749,7 +11274,10 @@
         <v>73</v>
       </c>
       <c r="C13" t="s">
-        <v>135</v>
+        <v>134</v>
+      </c>
+      <c r="D13" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -10760,10 +11288,13 @@
         <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>143</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>145</v>
+        <v>142</v>
+      </c>
+      <c r="D14" t="s">
+        <v>142</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -10774,10 +11305,13 @@
         <v>58</v>
       </c>
       <c r="C15" t="s">
-        <v>143</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>146</v>
+        <v>142</v>
+      </c>
+      <c r="D15" t="s">
+        <v>142</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -10788,33 +11322,39 @@
         <v>60</v>
       </c>
       <c r="C16" t="s">
-        <v>143</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="E16" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="D16" t="s">
+        <v>142</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="F16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B17" t="s">
         <v>61</v>
       </c>
       <c r="C17" t="s">
-        <v>143</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="E17" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="D17" t="s">
+        <v>142</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="F17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -10822,13 +11362,16 @@
         <v>62</v>
       </c>
       <c r="C18" t="s">
-        <v>143</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="D18" t="s">
+        <v>134</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -10836,47 +11379,56 @@
         <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>143</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="D19" t="s">
+        <v>134</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B20" t="s">
         <v>68</v>
       </c>
       <c r="C20" t="s">
-        <v>143</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="E20" t="s">
+        <v>142</v>
+      </c>
+      <c r="D20" t="s">
+        <v>142</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="F20" t="s">
+        <v>164</v>
+      </c>
+      <c r="G20" t="s">
         <v>165</v>
       </c>
-      <c r="F20" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>177</v>
       </c>
       <c r="B21" t="s">
         <v>70</v>
       </c>
       <c r="C21" t="s">
-        <v>143</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="D21" t="s">
+        <v>142</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -10884,30 +11436,36 @@
         <v>71</v>
       </c>
       <c r="C22" t="s">
-        <v>143</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="E22" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="D22" t="s">
+        <v>142</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="F22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>78</v>
       </c>
       <c r="C23" t="s">
-        <v>143</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="D23" t="s">
+        <v>142</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -10915,32 +11473,38 @@
         <v>88</v>
       </c>
       <c r="C24" t="s">
-        <v>143</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="D24" t="s">
+        <v>142</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B25" t="s">
         <v>89</v>
       </c>
       <c r="C25" t="s">
-        <v>143</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="E25" t="s">
-        <v>172</v>
+        <v>142</v>
+      </c>
+      <c r="D25" t="s">
+        <v>142</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="F25" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -10948,26 +11512,26 @@
     <sortCondition ref="C2:C25"/>
   </sortState>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C25" xr:uid="{1AF688A6-E6CD-4C08-9181-ACF0DEB89626}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C25 D3:D13" xr:uid="{1AF688A6-E6CD-4C08-9181-ACF0DEB89626}">
       <formula1>"Yes,No,N/A"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D14" r:id="rId1" xr:uid="{BD6B94F4-06B9-4404-A468-60E25E6425F0}"/>
-    <hyperlink ref="D15" r:id="rId2" xr:uid="{7D909D3A-1245-49CE-B04F-A449605E512B}"/>
-    <hyperlink ref="D16" r:id="rId3" xr:uid="{991712BE-2DAB-433E-B7F1-1736F0FA63FA}"/>
-    <hyperlink ref="D17" r:id="rId4" xr:uid="{7F9BDFFC-91E2-4241-B41B-C17461E2C2B4}"/>
-    <hyperlink ref="D18" r:id="rId5" xr:uid="{6F8FA59F-CEBE-440C-B910-037FB9729522}"/>
-    <hyperlink ref="D7" r:id="rId6" xr:uid="{05D694FD-20A6-4331-BA72-F002408A4734}"/>
-    <hyperlink ref="D19" r:id="rId7" xr:uid="{1249D900-31C7-47D0-A0CF-0F709CA92A3C}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{406FB329-6AB5-4462-9EA4-C8714AC37DC3}"/>
-    <hyperlink ref="D20" r:id="rId9" xr:uid="{DA06B138-B937-4E20-B62E-A90FAC325B11}"/>
-    <hyperlink ref="D21" r:id="rId10" xr:uid="{A62C92FB-C8D8-46D9-AB42-E372679F073E}"/>
-    <hyperlink ref="D22" r:id="rId11" xr:uid="{42F3A13A-56A9-4791-B05C-CBB1DFCDCFCC}"/>
-    <hyperlink ref="D23" r:id="rId12" xr:uid="{EAC90D7E-B3CB-42E5-80E2-92A373E1A09B}"/>
-    <hyperlink ref="D24" r:id="rId13" xr:uid="{1C66CEB9-4876-4BB8-A432-02FAE1D5C3BD}"/>
-    <hyperlink ref="D25" r:id="rId14" xr:uid="{016D0BC9-FC83-424E-AD4C-F36D6AF1414E}"/>
-    <hyperlink ref="D8" r:id="rId15" xr:uid="{4FA17220-086F-4CCC-A67F-A03213DF3CDC}"/>
+    <hyperlink ref="E14" r:id="rId1" xr:uid="{BD6B94F4-06B9-4404-A468-60E25E6425F0}"/>
+    <hyperlink ref="E15" r:id="rId2" xr:uid="{7D909D3A-1245-49CE-B04F-A449605E512B}"/>
+    <hyperlink ref="E16" r:id="rId3" xr:uid="{991712BE-2DAB-433E-B7F1-1736F0FA63FA}"/>
+    <hyperlink ref="E17" r:id="rId4" xr:uid="{7F9BDFFC-91E2-4241-B41B-C17461E2C2B4}"/>
+    <hyperlink ref="E18" r:id="rId5" xr:uid="{6F8FA59F-CEBE-440C-B910-037FB9729522}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{05D694FD-20A6-4331-BA72-F002408A4734}"/>
+    <hyperlink ref="E19" r:id="rId7" xr:uid="{1249D900-31C7-47D0-A0CF-0F709CA92A3C}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{406FB329-6AB5-4462-9EA4-C8714AC37DC3}"/>
+    <hyperlink ref="E20" r:id="rId9" xr:uid="{DA06B138-B937-4E20-B62E-A90FAC325B11}"/>
+    <hyperlink ref="E21" r:id="rId10" xr:uid="{A62C92FB-C8D8-46D9-AB42-E372679F073E}"/>
+    <hyperlink ref="E22" r:id="rId11" xr:uid="{42F3A13A-56A9-4791-B05C-CBB1DFCDCFCC}"/>
+    <hyperlink ref="E23" r:id="rId12" xr:uid="{EAC90D7E-B3CB-42E5-80E2-92A373E1A09B}"/>
+    <hyperlink ref="E24" r:id="rId13" xr:uid="{1C66CEB9-4876-4BB8-A432-02FAE1D5C3BD}"/>
+    <hyperlink ref="E25" r:id="rId14" xr:uid="{016D0BC9-FC83-424E-AD4C-F36D6AF1414E}"/>
+    <hyperlink ref="E8" r:id="rId15" xr:uid="{4FA17220-086F-4CCC-A67F-A03213DF3CDC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
@@ -11000,19 +11564,19 @@
         <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -11023,10 +11587,10 @@
         <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -11037,7 +11601,7 @@
         <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -11048,10 +11612,10 @@
         <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -11062,10 +11626,10 @@
         <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -11076,7 +11640,7 @@
         <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -11087,30 +11651,30 @@
         <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B8" t="s">
         <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="300" x14ac:dyDescent="0.25">
@@ -11121,10 +11685,10 @@
         <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -11135,21 +11699,21 @@
         <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B11" t="s">
         <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -11160,10 +11724,10 @@
         <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -11174,10 +11738,10 @@
         <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -11188,10 +11752,10 @@
         <v>64</v>
       </c>
       <c r="C14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -11202,10 +11766,10 @@
         <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -11216,7 +11780,7 @@
         <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -11224,10 +11788,10 @@
         <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -11238,27 +11802,27 @@
         <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B19" t="s">
         <v>68</v>
       </c>
       <c r="C19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E19" t="s">
+        <v>164</v>
+      </c>
+      <c r="F19" t="s">
         <v>165</v>
-      </c>
-      <c r="F19" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -11269,10 +11833,10 @@
         <v>70</v>
       </c>
       <c r="C20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -11283,13 +11847,13 @@
         <v>71</v>
       </c>
       <c r="C21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -11300,7 +11864,7 @@
         <v>73</v>
       </c>
       <c r="C22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -11311,10 +11875,10 @@
         <v>78</v>
       </c>
       <c r="C23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -11325,27 +11889,27 @@
         <v>88</v>
       </c>
       <c r="C24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B25" t="s">
         <v>89</v>
       </c>
       <c r="C25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -11399,10 +11963,10 @@
         <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -11421,7 +11985,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
         <v>68</v>
@@ -11435,7 +11999,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
         <v>68</v>
@@ -11449,7 +12013,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5" t="s">
         <v>68</v>
@@ -11477,10 +12041,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C7" t="s">
         <v>23</v>
@@ -11491,7 +12055,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B8" t="s">
         <v>89</v>
@@ -11612,7 +12176,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -11623,30 +12187,31 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BABF643E-67AC-4C76-84C9-66392C75839F}">
-  <dimension ref="A3:F109"/>
+  <dimension ref="A3:F129"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="F106" sqref="F106"/>
+    <sheetView topLeftCell="A101" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B134" sqref="B134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="49.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="49.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="56.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="16" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7.5703125" bestFit="1" customWidth="1"/>
@@ -12116,7 +12681,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -12150,7 +12715,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>94</v>
@@ -12161,13 +12726,13 @@
         <v>92</v>
       </c>
       <c r="B84" t="s">
+        <v>141</v>
+      </c>
+      <c r="C84" t="s">
+        <v>134</v>
+      </c>
+      <c r="D84" t="s">
         <v>142</v>
-      </c>
-      <c r="C84" t="s">
-        <v>135</v>
-      </c>
-      <c r="D84" t="s">
-        <v>143</v>
       </c>
       <c r="E84" t="s">
         <v>93</v>
@@ -12177,10 +12742,12 @@
       <c r="A85" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C85">
-        <v>1</v>
-      </c>
-      <c r="E85">
+      <c r="B85" s="10"/>
+      <c r="C85" s="10">
+        <v>1</v>
+      </c>
+      <c r="D85" s="10"/>
+      <c r="E85" s="10">
         <v>1</v>
       </c>
     </row>
@@ -12188,10 +12755,12 @@
       <c r="A86" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D86">
-        <v>1</v>
-      </c>
-      <c r="E86">
+      <c r="B86" s="10"/>
+      <c r="C86" s="10"/>
+      <c r="D86" s="10">
+        <v>1</v>
+      </c>
+      <c r="E86" s="10">
         <v>1</v>
       </c>
     </row>
@@ -12199,10 +12768,12 @@
       <c r="A87" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D87">
-        <v>1</v>
-      </c>
-      <c r="E87">
+      <c r="B87" s="10"/>
+      <c r="C87" s="10"/>
+      <c r="D87" s="10">
+        <v>1</v>
+      </c>
+      <c r="E87" s="10">
         <v>1</v>
       </c>
     </row>
@@ -12210,10 +12781,12 @@
       <c r="A88" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C88">
-        <v>1</v>
-      </c>
-      <c r="E88">
+      <c r="B88" s="10"/>
+      <c r="C88" s="10">
+        <v>1</v>
+      </c>
+      <c r="D88" s="10"/>
+      <c r="E88" s="10">
         <v>1</v>
       </c>
     </row>
@@ -12221,10 +12794,12 @@
       <c r="A89" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D89">
-        <v>1</v>
-      </c>
-      <c r="E89">
+      <c r="B89" s="10"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="10">
+        <v>1</v>
+      </c>
+      <c r="E89" s="10">
         <v>1</v>
       </c>
     </row>
@@ -12232,10 +12807,12 @@
       <c r="A90" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D90">
-        <v>1</v>
-      </c>
-      <c r="E90">
+      <c r="B90" s="10"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="10">
+        <v>1</v>
+      </c>
+      <c r="E90" s="10">
         <v>1</v>
       </c>
     </row>
@@ -12243,10 +12820,12 @@
       <c r="A91" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C91">
-        <v>1</v>
-      </c>
-      <c r="E91">
+      <c r="B91" s="10"/>
+      <c r="C91" s="10">
+        <v>1</v>
+      </c>
+      <c r="D91" s="10"/>
+      <c r="E91" s="10">
         <v>1</v>
       </c>
     </row>
@@ -12254,10 +12833,12 @@
       <c r="A92" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C92">
-        <v>1</v>
-      </c>
-      <c r="E92">
+      <c r="B92" s="10"/>
+      <c r="C92" s="10">
+        <v>1</v>
+      </c>
+      <c r="D92" s="10"/>
+      <c r="E92" s="10">
         <v>1</v>
       </c>
     </row>
@@ -12265,10 +12846,12 @@
       <c r="A93" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B93">
-        <v>1</v>
-      </c>
-      <c r="E93">
+      <c r="B93" s="10">
+        <v>1</v>
+      </c>
+      <c r="C93" s="10"/>
+      <c r="D93" s="10"/>
+      <c r="E93" s="10">
         <v>1</v>
       </c>
     </row>
@@ -12276,10 +12859,12 @@
       <c r="A94" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D94">
-        <v>1</v>
-      </c>
-      <c r="E94">
+      <c r="B94" s="10"/>
+      <c r="C94" s="10"/>
+      <c r="D94" s="10">
+        <v>1</v>
+      </c>
+      <c r="E94" s="10">
         <v>1</v>
       </c>
     </row>
@@ -12287,10 +12872,12 @@
       <c r="A95" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D95">
-        <v>1</v>
-      </c>
-      <c r="E95">
+      <c r="B95" s="10"/>
+      <c r="C95" s="10"/>
+      <c r="D95" s="10">
+        <v>1</v>
+      </c>
+      <c r="E95" s="10">
         <v>1</v>
       </c>
     </row>
@@ -12298,10 +12885,12 @@
       <c r="A96" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D96">
-        <v>1</v>
-      </c>
-      <c r="E96">
+      <c r="B96" s="10"/>
+      <c r="C96" s="10"/>
+      <c r="D96" s="10">
+        <v>1</v>
+      </c>
+      <c r="E96" s="10">
         <v>1</v>
       </c>
     </row>
@@ -12309,10 +12898,12 @@
       <c r="A97" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C97">
-        <v>1</v>
-      </c>
-      <c r="E97">
+      <c r="B97" s="10"/>
+      <c r="C97" s="10">
+        <v>1</v>
+      </c>
+      <c r="D97" s="10"/>
+      <c r="E97" s="10">
         <v>1</v>
       </c>
     </row>
@@ -12320,10 +12911,12 @@
       <c r="A98" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C98">
-        <v>1</v>
-      </c>
-      <c r="E98">
+      <c r="B98" s="10"/>
+      <c r="C98" s="10">
+        <v>1</v>
+      </c>
+      <c r="D98" s="10"/>
+      <c r="E98" s="10">
         <v>1</v>
       </c>
     </row>
@@ -12331,10 +12924,12 @@
       <c r="A99" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C99">
-        <v>1</v>
-      </c>
-      <c r="E99">
+      <c r="B99" s="10"/>
+      <c r="C99" s="10">
+        <v>1</v>
+      </c>
+      <c r="D99" s="10"/>
+      <c r="E99" s="10">
         <v>1</v>
       </c>
     </row>
@@ -12342,10 +12937,12 @@
       <c r="A100" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D100">
-        <v>1</v>
-      </c>
-      <c r="E100">
+      <c r="B100" s="10"/>
+      <c r="C100" s="10"/>
+      <c r="D100" s="10">
+        <v>1</v>
+      </c>
+      <c r="E100" s="10">
         <v>1</v>
       </c>
     </row>
@@ -12353,10 +12950,12 @@
       <c r="A101" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D101">
-        <v>1</v>
-      </c>
-      <c r="E101">
+      <c r="B101" s="10"/>
+      <c r="C101" s="10"/>
+      <c r="D101" s="10">
+        <v>1</v>
+      </c>
+      <c r="E101" s="10">
         <v>1</v>
       </c>
     </row>
@@ -12364,10 +12963,12 @@
       <c r="A102" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C102">
-        <v>1</v>
-      </c>
-      <c r="E102">
+      <c r="B102" s="10"/>
+      <c r="C102" s="10">
+        <v>1</v>
+      </c>
+      <c r="D102" s="10"/>
+      <c r="E102" s="10">
         <v>1</v>
       </c>
     </row>
@@ -12375,10 +12976,12 @@
       <c r="A103" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D103">
-        <v>1</v>
-      </c>
-      <c r="E103">
+      <c r="B103" s="10"/>
+      <c r="C103" s="10"/>
+      <c r="D103" s="10">
+        <v>1</v>
+      </c>
+      <c r="E103" s="10">
         <v>1</v>
       </c>
     </row>
@@ -12386,10 +12989,12 @@
       <c r="A104" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C104">
-        <v>1</v>
-      </c>
-      <c r="E104">
+      <c r="B104" s="10"/>
+      <c r="C104" s="10">
+        <v>1</v>
+      </c>
+      <c r="D104" s="10"/>
+      <c r="E104" s="10">
         <v>1</v>
       </c>
     </row>
@@ -12397,10 +13002,12 @@
       <c r="A105" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C105">
-        <v>1</v>
-      </c>
-      <c r="E105">
+      <c r="B105" s="10"/>
+      <c r="C105" s="10">
+        <v>1</v>
+      </c>
+      <c r="D105" s="10"/>
+      <c r="E105" s="10">
         <v>1</v>
       </c>
     </row>
@@ -12408,10 +13015,12 @@
       <c r="A106" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D106">
-        <v>1</v>
-      </c>
-      <c r="E106">
+      <c r="B106" s="10"/>
+      <c r="C106" s="10"/>
+      <c r="D106" s="10">
+        <v>1</v>
+      </c>
+      <c r="E106" s="10">
         <v>1</v>
       </c>
     </row>
@@ -12419,21 +13028,25 @@
       <c r="A107" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D107">
-        <v>1</v>
-      </c>
-      <c r="E107">
+      <c r="B107" s="10"/>
+      <c r="C107" s="10"/>
+      <c r="D107" s="10">
+        <v>1</v>
+      </c>
+      <c r="E107" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C108">
-        <v>1</v>
-      </c>
-      <c r="E108">
+        <v>105</v>
+      </c>
+      <c r="B108" s="10"/>
+      <c r="C108" s="10">
+        <v>1</v>
+      </c>
+      <c r="D108" s="10"/>
+      <c r="E108" s="10">
         <v>1</v>
       </c>
     </row>
@@ -12441,22 +13054,102 @@
       <c r="A109" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B109">
-        <v>1</v>
-      </c>
-      <c r="C109">
+      <c r="B109" s="10">
+        <v>1</v>
+      </c>
+      <c r="C109" s="10">
         <v>11</v>
       </c>
-      <c r="D109">
+      <c r="D109" s="10">
         <v>12</v>
       </c>
-      <c r="E109">
+      <c r="E109" s="10">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B116" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B117" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B118" s="10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B119" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B120" s="10">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B125" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B126" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B127" s="10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B128" s="10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B129" s="10">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
-  <drawing r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <drawing r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added meta and source information to some of the datasets
</commit_message>
<xml_diff>
--- a/robot_types.xlsx
+++ b/robot_types.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://connectqutedu-my.sharepoint.com/personal/tola_qut_edu_au/Documents/Desktop/gitrepos/urdf_analyzer/resources/urdf_files_dataset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dani-\Desktop\git_repos\urdf_analyzer\resources\urdf_files_dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="949" documentId="11_F25DC773A252ABDACC104829591E5E145ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9484EC17-7D4B-4FDC-9726-9954343F4A04}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE9D7E2-2DB9-44C8-BE5A-CAF5F3E614CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classification" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,8 @@
   <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId8"/>
-    <pivotCache cacheId="9" r:id="rId9"/>
-    <pivotCache cacheId="14" r:id="rId10"/>
+    <pivotCache cacheId="1" r:id="rId9"/>
+    <pivotCache cacheId="2" r:id="rId10"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -671,7 +671,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -690,7 +690,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -755,7 +754,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-DK"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -803,7 +802,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -859,7 +858,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -1041,7 +1040,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="862988239"/>
@@ -1100,7 +1099,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="862994895"/>
@@ -1142,7 +1141,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-DK"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1179,7 +1178,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-DK"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1250,7 +1249,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-DK"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1298,7 +1297,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -1354,7 +1353,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -1500,7 +1499,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1233920799"/>
@@ -1559,7 +1558,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1233923711"/>
@@ -1601,7 +1600,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-DK"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1638,7 +1637,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-DK"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1727,7 +1726,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -1783,7 +1782,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -1839,7 +1838,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -1895,7 +1894,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -1951,7 +1950,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2007,7 +2006,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2063,7 +2062,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2119,7 +2118,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2175,7 +2174,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2231,7 +2230,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2287,7 +2286,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2343,7 +2342,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2399,7 +2398,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2455,7 +2454,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2511,7 +2510,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2567,7 +2566,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2623,7 +2622,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2679,7 +2678,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2735,7 +2734,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2791,7 +2790,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2847,7 +2846,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2903,7 +2902,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2959,7 +2958,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3015,7 +3014,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3071,7 +3070,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3127,7 +3126,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3183,7 +3182,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3239,7 +3238,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3295,7 +3294,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3351,7 +3350,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3407,7 +3406,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3544,7 +3543,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3600,7 +3599,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3656,7 +3655,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3712,7 +3711,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3768,7 +3767,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3824,7 +3823,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3880,7 +3879,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3936,7 +3935,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -4592,7 +4591,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="852079311"/>
@@ -4651,7 +4650,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="852074735"/>
@@ -4693,7 +4692,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-DK"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4730,7 +4729,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-DK"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7858,540 +7857,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7DB9AB06-7A0B-43D1-8D65-CBF8CDFF313F}" name="PivotTable6" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A125:B129" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="25">
-        <item x="7"/>
-        <item x="18"/>
-        <item x="12"/>
-        <item x="1"/>
-        <item x="19"/>
-        <item x="21"/>
-        <item x="11"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="4"/>
-        <item x="6"/>
-        <item x="3"/>
-        <item x="23"/>
-        <item x="20"/>
-        <item x="5"/>
-        <item x="22"/>
-        <item x="8"/>
-        <item x="10"/>
-        <item x="17"/>
-        <item x="16"/>
-        <item x="9"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Manufacturer provides URDF file" fld="2" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7247F8BF-CB69-45E8-B510-8C11315D1775}" name="PivotTable5" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A116:B120" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="25">
-        <item x="7"/>
-        <item x="18"/>
-        <item x="12"/>
-        <item x="1"/>
-        <item x="19"/>
-        <item x="21"/>
-        <item x="11"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="4"/>
-        <item x="6"/>
-        <item x="3"/>
-        <item x="23"/>
-        <item x="20"/>
-        <item x="5"/>
-        <item x="22"/>
-        <item x="8"/>
-        <item x="10"/>
-        <item x="17"/>
-        <item x="16"/>
-        <item x="9"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Accessed" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="0" format="37" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7F910A06-381E-4205-8A11-C037FFB06F19}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A25:B30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="4">
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item x="3"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Type" fld="1" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BC3F2483-E8BF-4DBF-A164-60FE6E5E2B6B}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A3:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="4">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="11">
-        <item x="5"/>
-        <item x="1"/>
-        <item x="6"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="7"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="11">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Type" fld="1" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C8D76A50-2177-495E-9784-C4DC095E567F}" name="PivotTable4" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A83:E109" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="25">
-        <item x="7"/>
-        <item x="18"/>
-        <item x="12"/>
-        <item x="1"/>
-        <item x="19"/>
-        <item x="21"/>
-        <item x="11"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="4"/>
-        <item x="6"/>
-        <item x="3"/>
-        <item x="23"/>
-        <item x="20"/>
-        <item x="5"/>
-        <item x="22"/>
-        <item x="8"/>
-        <item x="10"/>
-        <item x="17"/>
-        <item x="16"/>
-        <item x="9"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" dataField="1" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="25">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i>
-      <x v="23"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Manufacturer provides URDF file" fld="1" subtotal="count" baseField="0" baseItem="1"/>
-  </dataFields>
-  <chartFormats count="3">
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="3" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{52084291-B8D7-48BB-BE93-50F506D1CFF2}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A48:F74" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
@@ -8864,6 +8329,540 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7DB9AB06-7A0B-43D1-8D65-CBF8CDFF313F}" name="PivotTable6" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A125:B129" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="25">
+        <item x="7"/>
+        <item x="18"/>
+        <item x="12"/>
+        <item x="1"/>
+        <item x="19"/>
+        <item x="21"/>
+        <item x="11"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item x="3"/>
+        <item x="23"/>
+        <item x="20"/>
+        <item x="5"/>
+        <item x="22"/>
+        <item x="8"/>
+        <item x="10"/>
+        <item x="17"/>
+        <item x="16"/>
+        <item x="9"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Manufacturer provides URDF file" fld="2" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7247F8BF-CB69-45E8-B510-8C11315D1775}" name="PivotTable5" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A116:B120" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="25">
+        <item x="7"/>
+        <item x="18"/>
+        <item x="12"/>
+        <item x="1"/>
+        <item x="19"/>
+        <item x="21"/>
+        <item x="11"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item x="3"/>
+        <item x="23"/>
+        <item x="20"/>
+        <item x="5"/>
+        <item x="22"/>
+        <item x="8"/>
+        <item x="10"/>
+        <item x="17"/>
+        <item x="16"/>
+        <item x="9"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Accessed" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="37" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7F910A06-381E-4205-8A11-C037FFB06F19}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A25:B30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="3"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Type" fld="1" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BC3F2483-E8BF-4DBF-A164-60FE6E5E2B6B}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A3:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="11">
+        <item x="5"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="7"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Type" fld="1" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C8D76A50-2177-495E-9784-C4DC095E567F}" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A83:E109" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="25">
+        <item x="7"/>
+        <item x="18"/>
+        <item x="12"/>
+        <item x="1"/>
+        <item x="19"/>
+        <item x="21"/>
+        <item x="11"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item x="3"/>
+        <item x="23"/>
+        <item x="20"/>
+        <item x="5"/>
+        <item x="22"/>
+        <item x="8"/>
+        <item x="10"/>
+        <item x="17"/>
+        <item x="16"/>
+        <item x="9"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" dataField="1" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="25">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Manufacturer provides URDF file" fld="1" subtotal="count" baseField="0" baseItem="1"/>
+  </dataFields>
+  <chartFormats count="3">
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -9129,7 +9128,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
@@ -11001,11 +11000,15 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H10:H11"/>
     <mergeCell ref="G12:G13"/>
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="F2:F3"/>
@@ -11019,15 +11022,11 @@
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="F18:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12094,7 +12093,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D436AF-4A5C-4F46-81DF-CC60230C3571}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -12742,12 +12741,10 @@
       <c r="A85" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B85" s="10"/>
-      <c r="C85" s="10">
-        <v>1</v>
-      </c>
-      <c r="D85" s="10"/>
-      <c r="E85" s="10">
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="E85">
         <v>1</v>
       </c>
     </row>
@@ -12755,12 +12752,10 @@
       <c r="A86" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B86" s="10"/>
-      <c r="C86" s="10"/>
-      <c r="D86" s="10">
-        <v>1</v>
-      </c>
-      <c r="E86" s="10">
+      <c r="D86">
+        <v>1</v>
+      </c>
+      <c r="E86">
         <v>1</v>
       </c>
     </row>
@@ -12768,12 +12763,10 @@
       <c r="A87" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B87" s="10"/>
-      <c r="C87" s="10"/>
-      <c r="D87" s="10">
-        <v>1</v>
-      </c>
-      <c r="E87" s="10">
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87">
         <v>1</v>
       </c>
     </row>
@@ -12781,12 +12774,10 @@
       <c r="A88" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B88" s="10"/>
-      <c r="C88" s="10">
-        <v>1</v>
-      </c>
-      <c r="D88" s="10"/>
-      <c r="E88" s="10">
+      <c r="C88">
+        <v>1</v>
+      </c>
+      <c r="E88">
         <v>1</v>
       </c>
     </row>
@@ -12794,12 +12785,10 @@
       <c r="A89" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B89" s="10"/>
-      <c r="C89" s="10"/>
-      <c r="D89" s="10">
-        <v>1</v>
-      </c>
-      <c r="E89" s="10">
+      <c r="D89">
+        <v>1</v>
+      </c>
+      <c r="E89">
         <v>1</v>
       </c>
     </row>
@@ -12807,12 +12796,10 @@
       <c r="A90" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B90" s="10"/>
-      <c r="C90" s="10"/>
-      <c r="D90" s="10">
-        <v>1</v>
-      </c>
-      <c r="E90" s="10">
+      <c r="D90">
+        <v>1</v>
+      </c>
+      <c r="E90">
         <v>1</v>
       </c>
     </row>
@@ -12820,12 +12807,10 @@
       <c r="A91" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B91" s="10"/>
-      <c r="C91" s="10">
-        <v>1</v>
-      </c>
-      <c r="D91" s="10"/>
-      <c r="E91" s="10">
+      <c r="C91">
+        <v>1</v>
+      </c>
+      <c r="E91">
         <v>1</v>
       </c>
     </row>
@@ -12833,12 +12818,10 @@
       <c r="A92" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B92" s="10"/>
-      <c r="C92" s="10">
-        <v>1</v>
-      </c>
-      <c r="D92" s="10"/>
-      <c r="E92" s="10">
+      <c r="C92">
+        <v>1</v>
+      </c>
+      <c r="E92">
         <v>1</v>
       </c>
     </row>
@@ -12846,12 +12829,10 @@
       <c r="A93" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B93" s="10">
-        <v>1</v>
-      </c>
-      <c r="C93" s="10"/>
-      <c r="D93" s="10"/>
-      <c r="E93" s="10">
+      <c r="B93">
+        <v>1</v>
+      </c>
+      <c r="E93">
         <v>1</v>
       </c>
     </row>
@@ -12859,12 +12840,10 @@
       <c r="A94" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B94" s="10"/>
-      <c r="C94" s="10"/>
-      <c r="D94" s="10">
-        <v>1</v>
-      </c>
-      <c r="E94" s="10">
+      <c r="D94">
+        <v>1</v>
+      </c>
+      <c r="E94">
         <v>1</v>
       </c>
     </row>
@@ -12872,12 +12851,10 @@
       <c r="A95" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B95" s="10"/>
-      <c r="C95" s="10"/>
-      <c r="D95" s="10">
-        <v>1</v>
-      </c>
-      <c r="E95" s="10">
+      <c r="D95">
+        <v>1</v>
+      </c>
+      <c r="E95">
         <v>1</v>
       </c>
     </row>
@@ -12885,12 +12862,10 @@
       <c r="A96" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B96" s="10"/>
-      <c r="C96" s="10"/>
-      <c r="D96" s="10">
-        <v>1</v>
-      </c>
-      <c r="E96" s="10">
+      <c r="D96">
+        <v>1</v>
+      </c>
+      <c r="E96">
         <v>1</v>
       </c>
     </row>
@@ -12898,12 +12873,10 @@
       <c r="A97" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B97" s="10"/>
-      <c r="C97" s="10">
-        <v>1</v>
-      </c>
-      <c r="D97" s="10"/>
-      <c r="E97" s="10">
+      <c r="C97">
+        <v>1</v>
+      </c>
+      <c r="E97">
         <v>1</v>
       </c>
     </row>
@@ -12911,12 +12884,10 @@
       <c r="A98" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B98" s="10"/>
-      <c r="C98" s="10">
-        <v>1</v>
-      </c>
-      <c r="D98" s="10"/>
-      <c r="E98" s="10">
+      <c r="C98">
+        <v>1</v>
+      </c>
+      <c r="E98">
         <v>1</v>
       </c>
     </row>
@@ -12924,12 +12895,10 @@
       <c r="A99" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B99" s="10"/>
-      <c r="C99" s="10">
-        <v>1</v>
-      </c>
-      <c r="D99" s="10"/>
-      <c r="E99" s="10">
+      <c r="C99">
+        <v>1</v>
+      </c>
+      <c r="E99">
         <v>1</v>
       </c>
     </row>
@@ -12937,12 +12906,10 @@
       <c r="A100" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B100" s="10"/>
-      <c r="C100" s="10"/>
-      <c r="D100" s="10">
-        <v>1</v>
-      </c>
-      <c r="E100" s="10">
+      <c r="D100">
+        <v>1</v>
+      </c>
+      <c r="E100">
         <v>1</v>
       </c>
     </row>
@@ -12950,12 +12917,10 @@
       <c r="A101" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B101" s="10"/>
-      <c r="C101" s="10"/>
-      <c r="D101" s="10">
-        <v>1</v>
-      </c>
-      <c r="E101" s="10">
+      <c r="D101">
+        <v>1</v>
+      </c>
+      <c r="E101">
         <v>1</v>
       </c>
     </row>
@@ -12963,12 +12928,10 @@
       <c r="A102" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B102" s="10"/>
-      <c r="C102" s="10">
-        <v>1</v>
-      </c>
-      <c r="D102" s="10"/>
-      <c r="E102" s="10">
+      <c r="C102">
+        <v>1</v>
+      </c>
+      <c r="E102">
         <v>1</v>
       </c>
     </row>
@@ -12976,12 +12939,10 @@
       <c r="A103" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B103" s="10"/>
-      <c r="C103" s="10"/>
-      <c r="D103" s="10">
-        <v>1</v>
-      </c>
-      <c r="E103" s="10">
+      <c r="D103">
+        <v>1</v>
+      </c>
+      <c r="E103">
         <v>1</v>
       </c>
     </row>
@@ -12989,12 +12950,10 @@
       <c r="A104" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B104" s="10"/>
-      <c r="C104" s="10">
-        <v>1</v>
-      </c>
-      <c r="D104" s="10"/>
-      <c r="E104" s="10">
+      <c r="C104">
+        <v>1</v>
+      </c>
+      <c r="E104">
         <v>1</v>
       </c>
     </row>
@@ -13002,12 +12961,10 @@
       <c r="A105" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B105" s="10"/>
-      <c r="C105" s="10">
-        <v>1</v>
-      </c>
-      <c r="D105" s="10"/>
-      <c r="E105" s="10">
+      <c r="C105">
+        <v>1</v>
+      </c>
+      <c r="E105">
         <v>1</v>
       </c>
     </row>
@@ -13015,12 +12972,10 @@
       <c r="A106" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B106" s="10"/>
-      <c r="C106" s="10"/>
-      <c r="D106" s="10">
-        <v>1</v>
-      </c>
-      <c r="E106" s="10">
+      <c r="D106">
+        <v>1</v>
+      </c>
+      <c r="E106">
         <v>1</v>
       </c>
     </row>
@@ -13028,12 +12983,10 @@
       <c r="A107" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B107" s="10"/>
-      <c r="C107" s="10"/>
-      <c r="D107" s="10">
-        <v>1</v>
-      </c>
-      <c r="E107" s="10">
+      <c r="D107">
+        <v>1</v>
+      </c>
+      <c r="E107">
         <v>1</v>
       </c>
     </row>
@@ -13041,12 +12994,10 @@
       <c r="A108" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B108" s="10"/>
-      <c r="C108" s="10">
-        <v>1</v>
-      </c>
-      <c r="D108" s="10"/>
-      <c r="E108" s="10">
+      <c r="C108">
+        <v>1</v>
+      </c>
+      <c r="E108">
         <v>1</v>
       </c>
     </row>
@@ -13054,16 +13005,16 @@
       <c r="A109" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B109" s="10">
-        <v>1</v>
-      </c>
-      <c r="C109" s="10">
+      <c r="B109">
+        <v>1</v>
+      </c>
+      <c r="C109">
         <v>11</v>
       </c>
-      <c r="D109" s="10">
+      <c r="D109">
         <v>12</v>
       </c>
-      <c r="E109" s="10">
+      <c r="E109">
         <v>24</v>
       </c>
     </row>
@@ -13079,7 +13030,7 @@
       <c r="A117" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B117" s="10">
+      <c r="B117">
         <v>1</v>
       </c>
     </row>
@@ -13087,7 +13038,7 @@
       <c r="A118" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B118" s="10">
+      <c r="B118">
         <v>13</v>
       </c>
     </row>
@@ -13095,7 +13046,7 @@
       <c r="A119" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B119" s="10">
+      <c r="B119">
         <v>10</v>
       </c>
     </row>
@@ -13103,7 +13054,7 @@
       <c r="A120" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B120" s="10">
+      <c r="B120">
         <v>24</v>
       </c>
     </row>
@@ -13119,7 +13070,7 @@
       <c r="A126" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B126" s="10">
+      <c r="B126">
         <v>1</v>
       </c>
     </row>
@@ -13127,7 +13078,7 @@
       <c r="A127" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B127" s="10">
+      <c r="B127">
         <v>11</v>
       </c>
     </row>
@@ -13135,7 +13086,7 @@
       <c r="A128" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B128" s="10">
+      <c r="B128">
         <v>12</v>
       </c>
     </row>
@@ -13143,7 +13094,7 @@
       <c r="A129" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B129" s="10">
+      <c r="B129">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added meta information to random dataset
</commit_message>
<xml_diff>
--- a/robot_types.xlsx
+++ b/robot_types.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dani-\Desktop\git_repos\urdf_analyzer\resources\urdf_files_dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tola\OneDrive - Queensland University of Technology\Desktop\gitrepos\urdf_analyzer\resources\urdf_files_dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE9D7E2-2DB9-44C8-BE5A-CAF5F3E614CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D4B133-5184-436A-8D06-E3801F00E226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classification" sheetId="1" r:id="rId1"/>
@@ -19,16 +19,17 @@
     <sheet name="Sheet1" sheetId="7" r:id="rId4"/>
     <sheet name="comparison with urdf from OEM" sheetId="6" r:id="rId5"/>
     <sheet name="information" sheetId="2" r:id="rId6"/>
-    <sheet name="analysis" sheetId="3" r:id="rId7"/>
+    <sheet name="robots" sheetId="8" r:id="rId7"/>
+    <sheet name="analysis" sheetId="3" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'urdf from manufacturers'!$A$1:$B$81</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId8"/>
-    <pivotCache cacheId="1" r:id="rId9"/>
-    <pivotCache cacheId="2" r:id="rId10"/>
+    <pivotCache cacheId="0" r:id="rId9"/>
+    <pivotCache cacheId="1" r:id="rId10"/>
+    <pivotCache cacheId="2" r:id="rId11"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="195">
   <si>
     <t>Robot</t>
   </si>
@@ -593,13 +594,55 @@
   </si>
   <si>
     <t>Kinova Mico M1N4S200</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>UR5e</t>
+  </si>
+  <si>
+    <t>Allegro hand - left</t>
+  </si>
+  <si>
+    <t>Allegro hand - right</t>
+  </si>
+  <si>
+    <t>end effector</t>
+  </si>
+  <si>
+    <t>Universal Robots</t>
+  </si>
+  <si>
+    <t>Wonik Robotics</t>
+  </si>
+  <si>
+    <t>Atlas - convex hull</t>
+  </si>
+  <si>
+    <t>Atlas - minimal contact</t>
+  </si>
+  <si>
+    <t>3F gripper</t>
+  </si>
+  <si>
+    <t>Robotiq</t>
+  </si>
+  <si>
+    <t>3F gripper - articulated</t>
+  </si>
+  <si>
+    <t>3F gripper - tendons</t>
+  </si>
+  <si>
+    <t>Kuk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -637,6 +680,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -671,7 +720,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -689,6 +738,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -754,7 +806,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-DK"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -802,7 +854,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -858,7 +910,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -1040,7 +1092,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="862988239"/>
@@ -1099,7 +1151,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="862994895"/>
@@ -1141,7 +1193,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-DK"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1178,7 +1230,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-DK"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1249,7 +1301,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-DK"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1297,7 +1349,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -1353,7 +1405,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -1499,7 +1551,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1233920799"/>
@@ -1558,7 +1610,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1233923711"/>
@@ -1600,7 +1652,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-DK"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1637,7 +1689,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-DK"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1726,7 +1778,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -1782,7 +1834,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -1838,7 +1890,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -1894,7 +1946,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -1950,7 +2002,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2006,7 +2058,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2062,7 +2114,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2118,7 +2170,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2174,7 +2226,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2230,7 +2282,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2286,7 +2338,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2342,7 +2394,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2398,7 +2450,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2454,7 +2506,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2510,7 +2562,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2566,7 +2618,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2622,7 +2674,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2678,7 +2730,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2734,7 +2786,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2790,7 +2842,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2846,7 +2898,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2902,7 +2954,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -2958,7 +3010,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3014,7 +3066,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3070,7 +3122,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3126,7 +3178,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3182,7 +3234,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3238,7 +3290,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3294,7 +3346,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3350,7 +3402,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3406,7 +3458,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3543,7 +3595,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3599,7 +3651,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3655,7 +3707,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3711,7 +3763,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3767,7 +3819,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3823,7 +3875,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3879,7 +3931,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3935,7 +3987,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -4591,7 +4643,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="852079311"/>
@@ -4650,7 +4702,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="852074735"/>
@@ -4692,7 +4744,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-DK"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4729,7 +4781,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-DK"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7857,6 +7909,195 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C8D76A50-2177-495E-9784-C4DC095E567F}" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A83:E109" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="25">
+        <item x="7"/>
+        <item x="18"/>
+        <item x="12"/>
+        <item x="1"/>
+        <item x="19"/>
+        <item x="21"/>
+        <item x="11"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item x="3"/>
+        <item x="23"/>
+        <item x="20"/>
+        <item x="5"/>
+        <item x="22"/>
+        <item x="8"/>
+        <item x="10"/>
+        <item x="17"/>
+        <item x="16"/>
+        <item x="9"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" dataField="1" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="25">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Manufacturer provides URDF file" fld="1" subtotal="count" baseField="0" baseItem="1"/>
+  </dataFields>
+  <chartFormats count="3">
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{52084291-B8D7-48BB-BE93-50F506D1CFF2}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A48:F74" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
@@ -8329,7 +8570,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7DB9AB06-7A0B-43D1-8D65-CBF8CDFF313F}" name="PivotTable6" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A125:B129" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
@@ -8418,7 +8659,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7247F8BF-CB69-45E8-B510-8C11315D1775}" name="PivotTable5" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A116:B120" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
@@ -8518,7 +8759,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7F910A06-381E-4205-8A11-C037FFB06F19}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A25:B30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
@@ -8584,7 +8825,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BC3F2483-E8BF-4DBF-A164-60FE6E5E2B6B}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
@@ -8657,195 +8898,6 @@
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C8D76A50-2177-495E-9784-C4DC095E567F}" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A83:E109" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="25">
-        <item x="7"/>
-        <item x="18"/>
-        <item x="12"/>
-        <item x="1"/>
-        <item x="19"/>
-        <item x="21"/>
-        <item x="11"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="4"/>
-        <item x="6"/>
-        <item x="3"/>
-        <item x="23"/>
-        <item x="20"/>
-        <item x="5"/>
-        <item x="22"/>
-        <item x="8"/>
-        <item x="10"/>
-        <item x="17"/>
-        <item x="16"/>
-        <item x="9"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" dataField="1" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="25">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i>
-      <x v="23"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Manufacturer provides URDF file" fld="1" subtotal="count" baseField="0" baseItem="1"/>
-  </dataFields>
-  <chartFormats count="3">
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="3" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
           </reference>
         </references>
       </pivotArea>
@@ -11000,15 +11052,11 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="F18:F19"/>
     <mergeCell ref="G12:G13"/>
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="F2:F3"/>
@@ -11022,11 +11070,15 @@
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="G10:G11"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H10:H11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12093,7 +12145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D436AF-4A5C-4F46-81DF-CC60230C3571}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -12185,6 +12237,131 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{960DFF13-A0DD-4A53-BDBB-16786924E633}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>193</v>
+      </c>
+      <c r="B9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>194</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BABF643E-67AC-4C76-84C9-66392C75839F}">
   <dimension ref="A3:F129"/>
   <sheetViews>

</xml_diff>